<commit_message>
added summary ranking table
</commit_message>
<xml_diff>
--- a/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Analysis/Original-Runs_overall_summary.xlsx
+++ b/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Analysis/Original-Runs_overall_summary.xlsx
@@ -1,52 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikki\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED1C6268-7657-4AAE-821F-A6E0B554BCB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="845"/>
+    <workbookView xWindow="7812" yWindow="0" windowWidth="15324" windowHeight="12336" tabRatio="845" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="29" r:id="rId1"/>
-    <sheet name="ranking" sheetId="30" r:id="rId2"/>
-    <sheet name="for box plot" sheetId="31" r:id="rId3"/>
-    <sheet name="b Constant" sheetId="1" r:id="rId4"/>
-    <sheet name="P constant" sheetId="26" r:id="rId5"/>
-    <sheet name="Pb constant" sheetId="27" r:id="rId6"/>
-    <sheet name="No constants" sheetId="28" r:id="rId7"/>
+    <sheet name="Table" sheetId="32" r:id="rId2"/>
+    <sheet name="ranking" sheetId="30" r:id="rId3"/>
+    <sheet name="for box plot" sheetId="31" r:id="rId4"/>
+    <sheet name="b Constant" sheetId="1" r:id="rId5"/>
+    <sheet name="P constant" sheetId="26" r:id="rId6"/>
+    <sheet name="Pb constant" sheetId="27" r:id="rId7"/>
+    <sheet name="No constants" sheetId="28" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Overall!$G$2</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Overall!$G$3:$G$23</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'for box plot'!$H$2:$H$22</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'for box plot'!$I$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'for box plot'!$I$2:$I$22</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'for box plot'!$J$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'for box plot'!$J$2:$J$22</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'for box plot'!$K$1</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'for box plot'!$K$2:$K$22</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'for box plot'!$H$2:$H$22</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'for box plot'!$I$2:$I$22</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'for box plot'!$J$2:$J$22</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Overall!$H$2</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'for box plot'!$K$2:$K$22</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'for box plot'!$H$2:$H$22</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'for box plot'!$I$2:$I$22</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'for box plot'!$J$2:$J$22</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'for box plot'!$K$2:$K$22</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'for box plot'!$H$2:$H$22</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'for box plot'!$I$2:$I$22</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'for box plot'!$J$2:$J$22</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'for box plot'!$K$2:$K$22</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Overall!$H$3:$H$23</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Overall!$I$2</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Overall!$I$3:$I$23</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Overall!$J$2</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Overall!$J$3:$J$23</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'for box plot'!#REF!</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'for box plot'!$H$1</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -67,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="48">
   <si>
     <t>Trial</t>
   </si>
@@ -194,12 +180,221 @@
   <si>
     <t>Whisker-</t>
   </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Estimate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>P, b, w</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Estimate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">P </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> w b </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> held constant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Estimate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">b </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>w</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">P </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>held constant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Estimate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>w</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">P </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">b </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> held constant</t>
+    </r>
+  </si>
+  <si>
+    <t>XS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="173" formatCode="0.0000E+00"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +437,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -269,12 +485,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -284,7 +515,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -292,13 +523,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -320,7 +562,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -451,7 +693,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3495-4B1A-A683-934686B44C2F}"/>
             </c:ext>
@@ -526,7 +768,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3495-4B1A-A683-934686B44C2F}"/>
             </c:ext>
@@ -649,7 +891,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3495-4B1A-A683-934686B44C2F}"/>
             </c:ext>
@@ -727,7 +969,7 @@
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
@@ -769,7 +1011,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -808,7 +1050,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -817,6 +1058,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -999,7 +1260,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3AE6-4C22-9488-42930035D488}"/>
             </c:ext>
@@ -1138,7 +1399,7 @@
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
@@ -2934,7 +3195,7 @@
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns="" Requires="cx1">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="7" name="Chart 6">
@@ -2960,15 +3221,15 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="Rectangle 1"/>
+            <xdr:cNvPr id="0" name=""/>
             <xdr:cNvSpPr>
               <a:spLocks noTextEdit="1"/>
             </xdr:cNvSpPr>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7767637" y="404812"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="7954327" y="389572"/>
+              <a:ext cx="4572000" cy="2636520"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3021,7 +3282,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4E7BC476-EEF9-2352-E7D5-C70DFEA5299D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E7BC476-EEF9-2352-E7D5-C70DFEA5299D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3062,7 +3323,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6F86DA50-4012-DB17-F88E-613B20E279DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F86DA50-4012-DB17-F88E-613B20E279DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3392,33 +3653,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -3426,7 +3687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3455,7 +3716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3488,7 +3749,7 @@
         <v>0.99943921155808202</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3521,7 +3782,7 @@
         <v>0.57378199452994139</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3554,7 +3815,7 @@
         <v>-8.07390872678317</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3587,7 +3848,7 @@
         <v>-7.6201871119879918</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3620,7 +3881,7 @@
         <v>-10.364264795735263</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3653,7 +3914,7 @@
         <v>-9.3694925286758508</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3686,7 +3947,7 @@
         <v>-9.5709960414292219</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3719,7 +3980,7 @@
         <v>-10.406762464391477</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3752,7 +4013,7 @@
         <v>-10.204729066973876</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3785,7 +4046,7 @@
         <v>-11.771428807063121</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3818,7 +4079,7 @@
         <v>-2.5011742318715036</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3851,7 +4112,7 @@
         <v>-9.3068304008574128</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3884,7 +4145,7 @@
         <v>-9.1896468299644258</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3917,7 +4178,7 @@
         <v>0.65322297963939147</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3950,7 +4211,7 @@
         <v>-11.073425277910742</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3983,7 +4244,7 @@
         <v>-9.8727550896682619</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4016,7 +4277,7 @@
         <v>0.65320442097495646</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4049,7 +4310,7 @@
         <v>0.87314717474368997</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4082,7 +4343,7 @@
         <v>-10.872421752369895</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4115,7 +4376,7 @@
         <v>-8.8941499598202505</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4148,7 +4409,7 @@
         <v>-8.4672656146057133</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4181,7 +4442,7 @@
         <v>-9.1000292137840564</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="2" customFormat="1">
+    <row r="25" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
@@ -4218,7 +4479,7 @@
         <v>-6.9503032787475538</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="2" customFormat="1" ht="15">
+    <row r="26" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>3</v>
       </c>
@@ -4263,42 +4524,625 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440A7D18-7A25-47C8-9799-855151A1FBA1}">
+  <dimension ref="A1:U23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="42.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>10</v>
+      </c>
+      <c r="C2" s="9">
+        <v>2.0856817999999999E-2</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1.02433E-7</v>
+      </c>
+      <c r="E2" s="10">
+        <v>3.6031300000000003E-8</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1.6926700000000001E-12</v>
+      </c>
+      <c r="G2" s="9">
+        <f>SUM(C2:F2)</f>
+        <v>2.0856956465992667E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>9</v>
+      </c>
+      <c r="C3" s="9">
+        <v>6.5284122E-2</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1.33007E-6</v>
+      </c>
+      <c r="E3" s="10">
+        <v>9.2077699999999999E-9</v>
+      </c>
+      <c r="F3" s="10">
+        <v>6.2412399999999997E-11</v>
+      </c>
+      <c r="G3" s="9">
+        <f>SUM(C3:F3)</f>
+        <v>6.5285461340182399E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>20</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.64156040199999997</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.198150831</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1.74914E-9</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1.2759999999999999E-9</v>
+      </c>
+      <c r="G4" s="9">
+        <f>SUM(C4:F4)</f>
+        <v>0.83971123602513997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1.553205822</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2.4502600000000002E-4</v>
+      </c>
+      <c r="E5" s="10">
+        <v>3.4340500000000002E-8</v>
+      </c>
+      <c r="F5" s="10">
+        <v>8.4351199999999993E-9</v>
+      </c>
+      <c r="G5" s="9">
+        <f>SUM(C5:F5)</f>
+        <v>1.5534508907756199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>6</v>
+      </c>
+      <c r="C6" s="9">
+        <v>2.515817744</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.75997610500000001</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2.84907E-7</v>
+      </c>
+      <c r="F6" s="10">
+        <v>4.2707800000000002E-10</v>
+      </c>
+      <c r="G6" s="9">
+        <f>SUM(C6:F6)</f>
+        <v>3.2757941343340784</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2.1391358999999999E-2</v>
+      </c>
+      <c r="D7" s="9">
+        <v>3.7478403669999998</v>
+      </c>
+      <c r="E7" s="10">
+        <v>7.3397999999999996E-6</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1.34146E-11</v>
+      </c>
+      <c r="G7" s="9">
+        <f>SUM(C7:F7)</f>
+        <v>3.7692390658134141</v>
+      </c>
+      <c r="U7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9">
+        <v>2.2486088560000002</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1.964952687</v>
+      </c>
+      <c r="E8" s="10">
+        <v>8.1226099999999995E-10</v>
+      </c>
+      <c r="F8" s="10">
+        <v>3.9195599999999997E-11</v>
+      </c>
+      <c r="G8" s="9">
+        <f>SUM(C8:F8)</f>
+        <v>4.2135615438514566</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8">
+        <v>5</v>
+      </c>
+      <c r="C9" s="9">
+        <v>4.1162418000000001</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.23689189899999999</v>
+      </c>
+      <c r="E9" s="10">
+        <v>3.6303600000000002E-6</v>
+      </c>
+      <c r="F9" s="10">
+        <v>4.3224999999999998E-11</v>
+      </c>
+      <c r="G9" s="9">
+        <f>SUM(C9:F9)</f>
+        <v>4.353137329403225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9">
+        <v>3.8275664659999999</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2.3122863E-2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1.1925822189999999</v>
+      </c>
+      <c r="F10" s="10">
+        <v>3.4098399999999999E-9</v>
+      </c>
+      <c r="G10" s="9">
+        <f>SUM(C10:F10)</f>
+        <v>5.0432715514098403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8">
+        <v>12</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1.113756118</v>
+      </c>
+      <c r="D11" s="9">
+        <v>5.942932152</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1.1991900000000001E-9</v>
+      </c>
+      <c r="F11" s="10">
+        <v>4.9336599999999999E-10</v>
+      </c>
+      <c r="G11" s="9">
+        <f>SUM(C11:F11)</f>
+        <v>7.0566882716925567</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8">
+        <v>15</v>
+      </c>
+      <c r="C12" s="9">
+        <v>7.9774977999999996E-2</v>
+      </c>
+      <c r="D12" s="9">
+        <v>9.1071930600000002</v>
+      </c>
+      <c r="E12" s="10">
+        <v>8.6778699999999996E-11</v>
+      </c>
+      <c r="F12" s="10">
+        <v>8.4445200000000005E-12</v>
+      </c>
+      <c r="G12" s="9">
+        <f>SUM(C12:F12)</f>
+        <v>9.1869680380952232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8">
+        <v>4</v>
+      </c>
+      <c r="C13" s="9">
+        <v>4.5806138980000002</v>
+      </c>
+      <c r="D13" s="9">
+        <v>7.7363728209999998</v>
+      </c>
+      <c r="E13" s="10">
+        <v>3.04047E-6</v>
+      </c>
+      <c r="F13" s="10">
+        <v>2.3978000000000001E-8</v>
+      </c>
+      <c r="G13" s="9">
+        <f>SUM(C13:F13)</f>
+        <v>12.316989783447999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8">
+        <v>16</v>
+      </c>
+      <c r="C14" s="9">
+        <v>12.41832913</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1.67177E-6</v>
+      </c>
+      <c r="E14" s="10">
+        <v>4.6698299999999999E-11</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1.3404300000000001E-10</v>
+      </c>
+      <c r="G14" s="9">
+        <f>SUM(C14:F14)</f>
+        <v>12.418330801950743</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8">
+        <v>17</v>
+      </c>
+      <c r="C15" s="9">
+        <v>4.4742410159999997</v>
+      </c>
+      <c r="D15" s="9">
+        <v>2.67405E-7</v>
+      </c>
+      <c r="E15" s="9">
+        <v>4.5015572260000001</v>
+      </c>
+      <c r="F15" s="9">
+        <v>4.4999161460000003</v>
+      </c>
+      <c r="G15" s="9">
+        <f>SUM(C15:F15)</f>
+        <v>13.475714655405</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8">
+        <v>14</v>
+      </c>
+      <c r="C16" s="9">
+        <v>6.8499549880000004</v>
+      </c>
+      <c r="D16" s="9">
+        <v>3.7517900000000003E-9</v>
+      </c>
+      <c r="E16" s="9">
+        <v>4.4998625069999996</v>
+      </c>
+      <c r="F16" s="9">
+        <v>4.5001084450000004</v>
+      </c>
+      <c r="G16" s="9">
+        <f>SUM(C16:F16)</f>
+        <v>15.84992594375179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2</v>
+      </c>
+      <c r="C17" s="9">
+        <v>5.9285567019999998</v>
+      </c>
+      <c r="D17" s="9">
+        <v>2.918055388</v>
+      </c>
+      <c r="E17" s="9">
+        <v>4.3002266479999998</v>
+      </c>
+      <c r="F17" s="9">
+        <v>3.7478482199999998</v>
+      </c>
+      <c r="G17" s="9">
+        <f>SUM(C17:F17)</f>
+        <v>16.894686958000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8">
+        <v>18</v>
+      </c>
+      <c r="C18" s="9">
+        <v>8.8409890549999997</v>
+      </c>
+      <c r="D18" s="9">
+        <v>3.6687500000000001E-4</v>
+      </c>
+      <c r="E18" s="9">
+        <v>7.1053368109999999</v>
+      </c>
+      <c r="F18" s="9">
+        <v>7.4670175959999998</v>
+      </c>
+      <c r="G18" s="9">
+        <f>SUM(C18:F18)</f>
+        <v>23.413710336999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8">
+        <v>11</v>
+      </c>
+      <c r="C19" s="9">
+        <v>5.2996438589999997</v>
+      </c>
+      <c r="D19" s="9">
+        <v>25.025922980000001</v>
+      </c>
+      <c r="E19" s="9">
+        <v>5.3388769999999997E-3</v>
+      </c>
+      <c r="F19" s="9">
+        <v>3.153739E-3</v>
+      </c>
+      <c r="G19" s="9">
+        <f>SUM(C19:F19)</f>
+        <v>30.334059454999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8">
+        <v>7</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.60187746399999997</v>
+      </c>
+      <c r="D20" s="9">
+        <v>32.959758049999998</v>
+      </c>
+      <c r="E20" s="10">
+        <v>4.5123700000000001E-10</v>
+      </c>
+      <c r="F20" s="10">
+        <v>2.6853700000000001E-10</v>
+      </c>
+      <c r="G20" s="9">
+        <f>SUM(C20:F20)</f>
+        <v>33.561635514719768</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8">
+        <v>13</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.27386723800000001</v>
+      </c>
+      <c r="D21" s="9">
+        <v>33.309229459999997</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1.0115299999999999E-9</v>
+      </c>
+      <c r="F21" s="10">
+        <v>6.4617900000000003E-10</v>
+      </c>
+      <c r="G21" s="9">
+        <f>SUM(C21:F21)</f>
+        <v>33.583096699657709</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9">
+        <v>26.96019235</v>
+      </c>
+      <c r="D22" s="9">
+        <v>22.4203601</v>
+      </c>
+      <c r="E22" s="9">
+        <v>9.9181798459999992</v>
+      </c>
+      <c r="F22" s="9">
+        <v>9.9870957019999995</v>
+      </c>
+      <c r="G22" s="9">
+        <f>SUM(C22:F22)</f>
+        <v>69.285827998000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8">
+        <v>22</v>
+      </c>
+      <c r="C23" s="9">
+        <v>4.9844587770000004</v>
+      </c>
+      <c r="D23" s="9">
+        <v>172.89238739999999</v>
+      </c>
+      <c r="E23" s="10">
+        <v>2.5939999999999999E-9</v>
+      </c>
+      <c r="F23" s="10">
+        <v>7.9427500000000003E-10</v>
+      </c>
+      <c r="G23" s="9">
+        <f>SUM(C23:F23)</f>
+        <v>177.87684618038827</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G23">
+    <sortCondition ref="G2:G23"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G2:G23" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH69"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2:J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="23" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="30" max="34" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="15">
+    <row r="1" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4396,7 +5240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="15">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4496,7 +5340,7 @@
         <v>2.0856956113064699E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="15">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4517,7 +5361,7 @@
         <v>4.2236717393228522</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G23" si="0">SUM(B3:E3)</f>
+        <f t="shared" ref="G3:G22" si="0">SUM(B3:E3)</f>
         <v>16.894686957291409</v>
       </c>
       <c r="I3">
@@ -4596,7 +5440,7 @@
         <v>9.1869680377084091</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="15">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4613,7 +5457,7 @@
         <v>8.4351201529012733E-9</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F3:F23" si="1">AVERAGE(B4:E4)</f>
+        <f t="shared" ref="F4:F23" si="1">AVERAGE(B4:E4)</f>
         <v>0.3883627226582182</v>
       </c>
       <c r="G4">
@@ -4696,7 +5540,7 @@
         <v>13.475714656006426</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="15">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4796,7 +5640,7 @@
         <v>33.561635517117907</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="15">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4896,7 +5740,7 @@
         <v>69.285828002278123</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="15">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4996,7 +5840,7 @@
         <v>12.418330806592964</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="15">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5096,7 +5940,7 @@
         <v>16.894686957291409</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="15">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5196,7 +6040,7 @@
         <v>33.583096695233294</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="15">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5296,7 +6140,7 @@
         <v>3.2757941339225507</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="15">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5396,7 +6240,7 @@
         <v>7.0566882716431838</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="15">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5496,7 +6340,7 @@
         <v>0.83971123597809472</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="15">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5596,7 +6440,7 @@
         <v>5.0432715509155956</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="15">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5696,7 +6540,7 @@
         <v>1.5534508906328728</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="15">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5796,7 +6640,7 @@
         <v>12.316989783527216</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="15">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5896,7 +6740,7 @@
         <v>30.334059455562144</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="15">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5994,7 +6838,7 @@
         <v>14.572721282153191</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="15">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6094,7 +6938,7 @@
         <v>15.849925943535156</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="15">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6194,7 +7038,7 @@
         <v>4.3531373295815516</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="15">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6294,7 +7138,7 @@
         <v>13.769231726436663</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="15">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -6394,7 +7238,7 @@
         <v>6.5285461842828296E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="15">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6494,7 +7338,7 @@
         <v>4.2135615431146247</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="15">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6531,8 +7375,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="15"/>
-    <row r="25" spans="1:34" ht="15">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -6603,7 +7446,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="15">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10</v>
       </c>
@@ -6681,7 +7524,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="15">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8</v>
       </c>
@@ -6759,7 +7602,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="15">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>12</v>
       </c>
@@ -6837,7 +7680,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="15">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -6915,7 +7758,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="15">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="L30">
         <v>5</v>
       </c>
@@ -6970,7 +7813,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="15">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="L31">
         <v>6</v>
       </c>
@@ -7025,7 +7868,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="15">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="L32">
         <v>7</v>
       </c>
@@ -7080,7 +7923,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="12:28" ht="15">
+    <row r="33" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L33">
         <v>8</v>
       </c>
@@ -7135,7 +7978,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="12:28" ht="15">
+    <row r="34" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L34">
         <v>9</v>
       </c>
@@ -7190,7 +8033,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="12:28" ht="15">
+    <row r="35" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L35">
         <v>10</v>
       </c>
@@ -7245,7 +8088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="12:28" ht="15">
+    <row r="36" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L36">
         <v>11</v>
       </c>
@@ -7300,7 +8143,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="12:28" ht="15">
+    <row r="37" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L37">
         <v>12</v>
       </c>
@@ -7355,7 +8198,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="12:28" ht="15">
+    <row r="38" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L38">
         <v>13</v>
       </c>
@@ -7410,7 +8253,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="12:28" ht="15">
+    <row r="39" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L39">
         <v>14</v>
       </c>
@@ -7465,7 +8308,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="12:28" ht="15">
+    <row r="40" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L40">
         <v>15</v>
       </c>
@@ -7520,7 +8363,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="12:28" ht="15">
+    <row r="41" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L41">
         <v>16</v>
       </c>
@@ -7575,7 +8418,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="12:28" ht="15">
+    <row r="42" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L42">
         <v>17</v>
       </c>
@@ -7630,7 +8473,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="12:28" ht="15">
+    <row r="43" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L43">
         <v>18</v>
       </c>
@@ -7685,7 +8528,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="12:28" ht="15">
+    <row r="44" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L44">
         <v>19</v>
       </c>
@@ -7740,7 +8583,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="12:28" ht="15">
+    <row r="45" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L45">
         <v>20</v>
       </c>
@@ -7795,7 +8638,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="12:28" ht="15">
+    <row r="46" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L46">
         <v>21</v>
       </c>
@@ -7850,7 +8693,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="12:28" ht="15">
+    <row r="48" spans="12:28" x14ac:dyDescent="0.3">
       <c r="L48" s="2" t="s">
         <v>0</v>
       </c>
@@ -7876,7 +8719,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="12:19" ht="15">
+    <row r="49" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L49">
         <v>10</v>
       </c>
@@ -7902,7 +8745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="12:19" ht="15">
+    <row r="50" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L50">
         <v>9</v>
       </c>
@@ -7928,7 +8771,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="12:19" ht="15">
+    <row r="51" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L51">
         <v>15</v>
       </c>
@@ -7954,7 +8797,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="12:19" ht="15">
+    <row r="52" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L52">
         <v>8</v>
       </c>
@@ -7980,7 +8823,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="12:19" ht="15">
+    <row r="53" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L53">
         <v>19</v>
       </c>
@@ -8006,7 +8849,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="12:19">
+    <row r="54" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L54">
         <v>16</v>
       </c>
@@ -8032,7 +8875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="12:19">
+    <row r="55" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L55">
         <v>20</v>
       </c>
@@ -8058,7 +8901,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="12:19">
+    <row r="56" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L56">
         <v>7</v>
       </c>
@@ -8084,7 +8927,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="12:19">
+    <row r="57" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L57">
         <v>3</v>
       </c>
@@ -8110,7 +8953,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="12:19">
+    <row r="58" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L58">
         <v>12</v>
       </c>
@@ -8136,7 +8979,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="12:19">
+    <row r="59" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L59">
         <v>5</v>
       </c>
@@ -8162,7 +9005,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="12:19">
+    <row r="60" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L60">
         <v>6</v>
       </c>
@@ -8188,7 +9031,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="12:19">
+    <row r="61" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L61">
         <v>13</v>
       </c>
@@ -8214,7 +9057,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="12:19">
+    <row r="62" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L62">
         <v>21</v>
       </c>
@@ -8240,7 +9083,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="12:19">
+    <row r="63" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L63">
         <v>17</v>
       </c>
@@ -8266,7 +9109,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="12:19">
+    <row r="64" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L64">
         <v>14</v>
       </c>
@@ -8292,7 +9135,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="12:19">
+    <row r="65" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L65">
         <v>4</v>
       </c>
@@ -8318,7 +9161,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="12:19">
+    <row r="66" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L66">
         <v>18</v>
       </c>
@@ -8344,7 +9187,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="12:19">
+    <row r="67" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L67">
         <v>2</v>
       </c>
@@ -8370,7 +9213,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="12:19">
+    <row r="68" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L68">
         <v>11</v>
       </c>
@@ -8396,7 +9239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="12:19">
+    <row r="69" spans="12:19" x14ac:dyDescent="0.3">
       <c r="L69">
         <v>1</v>
       </c>
@@ -8423,7 +9266,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="I2:K23">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:K23">
     <sortCondition ref="K2:K23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8433,22 +9276,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8465,7 +9308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8482,7 +9325,7 @@
         <v>9.9870957021480429</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8499,7 +9342,7 @@
         <v>3.7478482197808591</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8516,7 +9359,7 @@
         <v>8.4351201529012733E-9</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8533,7 +9376,7 @@
         <v>2.3977996253966481E-8</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8550,7 +9393,7 @@
         <v>4.3225020136638796E-11</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8567,7 +9410,7 @@
         <v>4.2707826655854999E-10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8584,7 +9427,7 @@
         <v>2.6853689225398418E-10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -8601,7 +9444,7 @@
         <v>3.9195619734684774E-11</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -8618,7 +9461,7 @@
         <v>6.2412407158026194E-11</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -8635,7 +9478,7 @@
         <v>1.6926656966503639E-12</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -8652,7 +9495,7 @@
         <v>3.1537391407770736E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -8669,7 +9512,7 @@
         <v>4.9336643405195255E-10</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -8686,7 +9529,7 @@
         <v>6.4617949121827165E-10</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -8703,7 +9546,7 @@
         <v>4.500108444748113</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -8720,7 +9563,7 @@
         <v>8.444515206463839E-12</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -8737,24 +9580,24 @@
         <v>1.3404323801768158E-10</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="7">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18">
         <v>4.4742410164453847</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18">
         <v>2.6740527757220348E-7</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18">
         <v>4.5015572260013741</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18">
         <v>4.4999161461543888</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -8771,7 +9614,7 @@
         <v>7.4670175960146183</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -8788,7 +9631,7 @@
         <v>1.3414616072216297E-11</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -8805,7 +9648,7 @@
         <v>1.2759981366433912E-9</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8822,7 +9665,7 @@
         <v>3.409843017575834E-9</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>6</v>
       </c>
@@ -8836,7 +9679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -8857,7 +9700,7 @@
         <v>1.6926656966503639E-12</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -8878,7 +9721,7 @@
         <v>6.2412407158026194E-11</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -8899,7 +9742,7 @@
         <v>6.4617949121827165E-10</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -8920,7 +9763,7 @@
         <v>3.1537391407770736E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -8941,7 +9784,7 @@
         <v>9.9870957021480429</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
@@ -8955,7 +9798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -8976,7 +9819,7 @@
         <v>6.2412407158026194E-11</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -8997,7 +9840,7 @@
         <v>5.8376708406024546E-10</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -9018,7 +9861,7 @@
         <v>3.1537384945975822E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -9039,7 +9882,7 @@
         <v>9.9839419630072666</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -9066,21 +9909,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="15">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9094,7 +9937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>14</v>
       </c>
@@ -9108,7 +9951,7 @@
         <v>22.420360101114447</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -9122,7 +9965,7 @@
         <v>2.9180553881637055</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>17</v>
       </c>
@@ -9136,7 +9979,7 @@
         <v>2.4502578370133929E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>9</v>
       </c>
@@ -9150,7 +9993,7 @@
         <v>7.7363728209545508</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>16</v>
       </c>
@@ -9164,7 +10007,7 @@
         <v>0.23689189903145005</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -9178,7 +10021,7 @@
         <v>0.75997610472545973</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>18</v>
       </c>
@@ -9192,7 +10035,7 @@
         <v>32.959758052089796</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>21</v>
       </c>
@@ -9206,7 +10049,7 @@
         <v>1.9649526865915972</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>20</v>
       </c>
@@ -9220,7 +10063,7 @@
         <v>1.3300734061349089E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -9234,7 +10077,7 @@
         <v>1.0243273573452971E-7</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -9248,7 +10091,7 @@
         <v>25.025922980248851</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -9262,7 +10105,7 @@
         <v>5.9429321520069891</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -9276,7 +10119,7 @@
         <v>33.309229455397286</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>19</v>
       </c>
@@ -9290,7 +10133,7 @@
         <v>3.7517894224305708E-9</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -9304,7 +10147,7 @@
         <v>9.1071930599002631</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -9318,7 +10161,7 @@
         <v>1.6717735944856615E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -9332,7 +10175,7 @@
         <v>2.6740527757220348E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -9346,7 +10189,7 @@
         <v>3.6687489843564814E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>11</v>
       </c>
@@ -9360,7 +10203,7 @@
         <v>3.7478403669788567</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>7</v>
       </c>
@@ -9374,7 +10217,7 @@
         <v>0.19815083139884221</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>13</v>
       </c>
@@ -9388,7 +10231,7 @@
         <v>2.3122862555122112E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -9402,7 +10245,7 @@
         <v>172.89238739626737</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>2</v>
       </c>
@@ -9411,7 +10254,7 @@
         <v>14.511080065161069</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>3</v>
       </c>
@@ -9421,7 +10264,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="D2:E22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E22">
     <sortCondition ref="D2:D22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9429,17 +10272,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E2:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9453,7 +10296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>16</v>
       </c>
@@ -9467,7 +10310,7 @@
         <v>9.9181798458956543</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>15</v>
       </c>
@@ -9481,7 +10324,7 @@
         <v>4.3002266476297253</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7</v>
       </c>
@@ -9495,7 +10338,7 @@
         <v>3.4340534828846362E-8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
@@ -9509,7 +10352,7 @@
         <v>3.0404652118011022E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>13</v>
       </c>
@@ -9523,7 +10366,7 @@
         <v>3.6303566876897907E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>12</v>
       </c>
@@ -9537,7 +10380,7 @@
         <v>2.8490723934436047E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20</v>
       </c>
@@ -9551,7 +10394,7 @@
         <v>4.5123729600762591E-10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>22</v>
       </c>
@@ -9565,7 +10408,7 @@
         <v>8.1226108532573268E-10</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9579,7 +10422,7 @@
         <v>9.2077725948340428E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -9593,7 +10436,7 @@
         <v>3.6031259077816692E-8</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -9607,7 +10450,7 @@
         <v>5.3388772082334952E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -9621,7 +10464,7 @@
         <v>1.1991863700778435E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
@@ -9635,7 +10478,7 @@
         <v>1.0115308916029265E-9</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
@@ -9649,7 +10492,7 @@
         <v>4.4998625069898432</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>19</v>
       </c>
@@ -9663,7 +10506,7 @@
         <v>8.6778700869389412E-11</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>11</v>
       </c>
@@ -9677,7 +10520,7 @@
         <v>4.6698300773274395E-11</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>21</v>
       </c>
@@ -9691,7 +10534,7 @@
         <v>4.5015572260013741</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -9705,7 +10548,7 @@
         <v>7.1053368112401367</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>14</v>
       </c>
@@ -9719,7 +10562,7 @@
         <v>7.3397955041235052E-6</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17</v>
       </c>
@@ -9733,7 +10576,7 @@
         <v>1.7491420541030022E-9</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>18</v>
       </c>
@@ -9747,7 +10590,7 @@
         <v>1.1925822189679345</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -9761,7 +10604,7 @@
         <v>2.5939981710941708E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>2</v>
       </c>
@@ -9769,7 +10612,7 @@
         <v>1.4328681144085429</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>3</v>
       </c>
@@ -9778,24 +10621,24 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B24">
     <sortCondition ref="B2:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>10</v>
       </c>
@@ -9809,7 +10652,7 @@
         <v>9.9870957021480429</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>15</v>
       </c>
@@ -9823,7 +10666,7 @@
         <v>3.7478482197808591</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>19</v>
       </c>
@@ -9837,7 +10680,7 @@
         <v>8.4351201529012733E-9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
@@ -9851,7 +10694,7 @@
         <v>2.3977996253966481E-8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -9865,7 +10708,7 @@
         <v>4.3225020136638796E-11</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -9879,7 +10722,7 @@
         <v>4.2707826655854999E-10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>16</v>
       </c>
@@ -9893,7 +10736,7 @@
         <v>2.6853689225398418E-10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9907,7 +10750,7 @@
         <v>3.9195619734684774E-11</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -9921,7 +10764,7 @@
         <v>6.2412407158026194E-11</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>12</v>
       </c>
@@ -9935,7 +10778,7 @@
         <v>1.6926656966503639E-12</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>13</v>
       </c>
@@ -9949,7 +10792,7 @@
         <v>3.1537391407770736E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>22</v>
       </c>
@@ -9963,7 +10806,7 @@
         <v>4.9336643405195255E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>20</v>
       </c>
@@ -9977,7 +10820,7 @@
         <v>6.4617949121827165E-10</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>21</v>
       </c>
@@ -9991,7 +10834,7 @@
         <v>4.500108444748113</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -10005,7 +10848,7 @@
         <v>8.444515206463839E-12</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
@@ -10019,7 +10862,7 @@
         <v>1.3404323801768158E-10</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>11</v>
       </c>
@@ -10033,7 +10876,7 @@
         <v>4.4999161461543888</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -10047,7 +10890,7 @@
         <v>7.4670175960146183</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -10061,7 +10904,7 @@
         <v>1.3414616072216297E-11</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>14</v>
       </c>
@@ -10075,7 +10918,7 @@
         <v>1.2759981366433912E-9</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -10089,7 +10932,7 @@
         <v>3.409843017575834E-9</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -10103,7 +10946,7 @@
         <v>7.9427480426631953E-10</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>2</v>
       </c>
@@ -10111,7 +10954,7 @@
         <v>1.3729609040008008</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>3</v>
       </c>
@@ -10124,17 +10967,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10148,7 +10991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -10162,7 +11005,7 @@
         <v>26.960192353119982</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>19</v>
       </c>
@@ -10176,7 +11019,7 @@
         <v>5.9285567017171177</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>9</v>
       </c>
@@ -10190,7 +11033,7 @@
         <v>1.5532058220735163</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>15</v>
       </c>
@@ -10204,7 +11047,7 @@
         <v>4.5806138981294575</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>13</v>
       </c>
@@ -10218,7 +11061,7 @@
         <v>4.1162418001501893</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -10232,7 +11075,7 @@
         <v>2.5158177438627733</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20</v>
       </c>
@@ -10246,7 +11089,7 @@
         <v>0.60187746430833444</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>12</v>
       </c>
@@ -10260,7 +11103,7 @@
         <v>2.2486088556715709</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -10274,7 +11117,7 @@
         <v>6.5284122499237152E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -10288,7 +11131,7 @@
         <v>2.0856817647377221E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -10302,7 +11145,7 @@
         <v>5.2996438589642807</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>21</v>
       </c>
@@ -10316,7 +11159,7 @@
         <v>1.1137561179436419</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -10330,7 +11173,7 @@
         <v>0.27386723817829484</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>17</v>
       </c>
@@ -10344,7 +11187,7 @@
         <v>6.8499549880454111</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
@@ -10358,7 +11201,7 @@
         <v>7.977497771292312E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>22</v>
       </c>
@@ -10372,7 +11215,7 @@
         <v>12.418329134638627</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11</v>
       </c>
@@ -10386,7 +11229,7 @@
         <v>4.4742410164453847</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -10400,7 +11243,7 @@
         <v>8.8409890549749708</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>14</v>
       </c>
@@ -10414,7 +11257,7 @@
         <v>2.1391359444392161E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -10428,7 +11271,7 @@
         <v>0.64156040155411242</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>16</v>
       </c>
@@ -10442,7 +11285,7 @@
         <v>3.8275664659826956</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -10456,7 +11299,7 @@
         <v>4.9844587765954298</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>2</v>
       </c>
@@ -10464,7 +11307,7 @@
         <v>4.4280358622572615</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>3</v>
       </c>
@@ -10473,7 +11316,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B24">
     <sortCondition ref="B2:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10481,6 +11324,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008DB5B7ED115EF04980BBFAFC51672553" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43a679fe5cbd3b1dc01cea5b3bb6a16a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="070f1269-45c1-4463-99ba-5dc4e57c7dff" xmlns:ns4="7bf50b4b-6300-445a-aea1-306a2291592c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0963d0390b393dc53bf13ff5a8315f4" ns3:_="" ns4:_="">
     <xsd:import namespace="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
@@ -10675,24 +11535,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAD4690-B959-480E-AC59-DDDE87F8E768}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02EB7017-44D4-47C1-BB45-296DD07AFBB9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10709,22 +11570,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAD4690-B959-480E-AC59-DDDE87F8E768}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>